<commit_message>
Para agregar una columna en el archivo en excel.
</commit_message>
<xml_diff>
--- a/Data/test.xlsx
+++ b/Data/test.xlsx
@@ -4,26 +4,41 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Habitos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,16 +58,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -341,20 +373,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Número de Serie</t>
         </is>
@@ -365,37 +397,40 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="2" ht="15" customHeight="1" s="1">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>Leer ciencia ficción.</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="3" ht="15" customHeight="1" s="1">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>Ir al cine.</t>
         </is>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="4" ht="15" customHeight="1" s="1">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>Comer cosas raras una vez al mes.</t>
         </is>
       </c>
     </row>
+    <row r="1048576" ht="12.8" customHeight="1" s="1"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregar datos en la segunda columna del excel y ejemplo de tuplas.
</commit_message>
<xml_diff>
--- a/Data/test.xlsx
+++ b/Data/test.xlsx
@@ -68,14 +68,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +383,16 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
+  <cols>
+    <col width="18.89" customWidth="1" style="2" min="1" max="1"/>
+    <col width="11.52" customWidth="1" style="2" min="1024" max="1024"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="1">
+    <row r="1" ht="15" customHeight="1" s="3">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Número de Serie</t>
@@ -397,7 +404,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="1">
+    <row r="2" ht="15" customHeight="1" s="3">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -407,7 +414,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="1">
+    <row r="3" ht="15" customHeight="1" s="3">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -417,7 +424,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" s="1">
+    <row r="4" ht="15" customHeight="1" s="3">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
@@ -427,7 +434,7 @@
         </is>
       </c>
     </row>
-    <row r="1048576" ht="12.8" customHeight="1" s="1"/>
+    <row r="1048576" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>